<commit_message>
nieuwe wijken en enkele verbeteringen
Update wijken
* laten vallen afzonderlijke afhandeling Brussel bij GGW7, omdat we nu wijken in Brussel hebben
* toevoegen nieuwe wijken voor Brussel, closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/25
* toevoegen nieuwe wijken voor LI, WV en VB, closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/22

Varia
* update deelgemeente en deelgemeente2019 (zie #24)
* vervoerregio = #LEEG! in export vermijden door er een alfanumerieke variabele van te maken, closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/18
* gewest toegevoegd in onderwerp v9900_gebiedscode (closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/17)
* zorg dat er geen "gebied onbekend" een geometrie krijgt (dat kan indien de standsector aan gebied onbekend wordt toegewezen). Dat gebeurde bij ggw7 en deelgemeente, closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/23
</commit_message>
<xml_diff>
--- a/data_voor_swing/uploadfiles/ggw7_type.xlsx
+++ b/data_voor_swing/uploadfiles/ggw7_type.xlsx
@@ -1527,7 +1527,7 @@
         <v>1970.00</v>
       </c>
       <c r="D71" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="0" outlineLevel="0">
@@ -1543,7 +1543,7 @@
         <v>1970.00</v>
       </c>
       <c r="D72" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="0" outlineLevel="0">
@@ -1559,7 +1559,7 @@
         <v>1970.00</v>
       </c>
       <c r="D73" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="0" outlineLevel="0">
@@ -1575,7 +1575,7 @@
         <v>1970.00</v>
       </c>
       <c r="D74" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="0" outlineLevel="0">
@@ -1591,7 +1591,7 @@
         <v>1970.00</v>
       </c>
       <c r="D75" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="0" outlineLevel="0">
@@ -1607,7 +1607,7 @@
         <v>1970.00</v>
       </c>
       <c r="D76" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="0" outlineLevel="0">
@@ -1623,7 +1623,7 @@
         <v>1970.00</v>
       </c>
       <c r="D77" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="0" outlineLevel="0">
@@ -1639,7 +1639,7 @@
         <v>1970.00</v>
       </c>
       <c r="D78" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="0" outlineLevel="0">
@@ -1655,7 +1655,7 @@
         <v>1970.00</v>
       </c>
       <c r="D79" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="0" outlineLevel="0">
@@ -1671,7 +1671,7 @@
         <v>1970.00</v>
       </c>
       <c r="D80" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="0" outlineLevel="0">
@@ -1687,7 +1687,7 @@
         <v>1970.00</v>
       </c>
       <c r="D81" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="82" spans="1:4" s="0" outlineLevel="0">
@@ -1703,7 +1703,7 @@
         <v>1970.00</v>
       </c>
       <c r="D82" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="83" spans="1:4" s="0" outlineLevel="0">
@@ -1719,7 +1719,7 @@
         <v>1970.00</v>
       </c>
       <c r="D83" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="84" spans="1:4" s="0" outlineLevel="0">
@@ -1735,7 +1735,7 @@
         <v>1970.00</v>
       </c>
       <c r="D84" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="0" outlineLevel="0">
@@ -1751,7 +1751,7 @@
         <v>1970.00</v>
       </c>
       <c r="D85" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="86" spans="1:4" s="0" outlineLevel="0">
@@ -1767,7 +1767,7 @@
         <v>1970.00</v>
       </c>
       <c r="D86" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="87" spans="1:4" s="0" outlineLevel="0">
@@ -1783,7 +1783,7 @@
         <v>1970.00</v>
       </c>
       <c r="D87" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="88" spans="1:4" s="0" outlineLevel="0">
@@ -1799,7 +1799,7 @@
         <v>1970.00</v>
       </c>
       <c r="D88" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="89" spans="1:4" s="0" outlineLevel="0">
@@ -1815,7 +1815,7 @@
         <v>1970.00</v>
       </c>
       <c r="D89" s="8">
-        <v>3.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="90" spans="1:4" s="0" outlineLevel="0">
@@ -1831,7 +1831,7 @@
         <v>1970.00</v>
       </c>
       <c r="D90" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="0" outlineLevel="0">
@@ -1863,7 +1863,7 @@
         <v>1970.00</v>
       </c>
       <c r="D92" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="93" spans="1:4" s="0" outlineLevel="0">
@@ -1911,7 +1911,7 @@
         <v>1970.00</v>
       </c>
       <c r="D95" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="96" spans="1:4" s="0" outlineLevel="0">
@@ -1927,7 +1927,7 @@
         <v>1970.00</v>
       </c>
       <c r="D96" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="0" outlineLevel="0">
@@ -1959,7 +1959,7 @@
         <v>1970.00</v>
       </c>
       <c r="D98" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="0" outlineLevel="0">
@@ -1975,7 +1975,7 @@
         <v>1970.00</v>
       </c>
       <c r="D99" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="0" outlineLevel="0">
@@ -1991,7 +1991,7 @@
         <v>1970.00</v>
       </c>
       <c r="D100" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="0" outlineLevel="0">
@@ -2039,7 +2039,7 @@
         <v>1970.00</v>
       </c>
       <c r="D103" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="104" spans="1:4" s="0" outlineLevel="0">
@@ -2071,7 +2071,7 @@
         <v>1970.00</v>
       </c>
       <c r="D105" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="106" spans="1:4" s="0" outlineLevel="0">
@@ -2087,7 +2087,7 @@
         <v>1970.00</v>
       </c>
       <c r="D106" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="0" outlineLevel="0">
@@ -2167,7 +2167,7 @@
         <v>1970.00</v>
       </c>
       <c r="D111" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="0" outlineLevel="0">
@@ -2199,7 +2199,7 @@
         <v>1970.00</v>
       </c>
       <c r="D113" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="114" spans="1:4" s="0" outlineLevel="0">
@@ -2215,7 +2215,7 @@
         <v>1970.00</v>
       </c>
       <c r="D114" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="115" spans="1:4" s="0" outlineLevel="0">
@@ -2231,7 +2231,7 @@
         <v>1970.00</v>
       </c>
       <c r="D115" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="116" spans="1:4" s="0" outlineLevel="0">
@@ -2359,7 +2359,7 @@
         <v>1970.00</v>
       </c>
       <c r="D123" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="124" spans="1:4" s="0" outlineLevel="0">
@@ -2391,7 +2391,7 @@
         <v>1970.00</v>
       </c>
       <c r="D125" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="126" spans="1:4" s="0" outlineLevel="0">
@@ -2407,7 +2407,7 @@
         <v>1970.00</v>
       </c>
       <c r="D126" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="127" spans="1:4" s="0" outlineLevel="0">
@@ -2423,7 +2423,7 @@
         <v>1970.00</v>
       </c>
       <c r="D127" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="128" spans="1:4" s="0" outlineLevel="0">
@@ -2455,7 +2455,7 @@
         <v>1970.00</v>
       </c>
       <c r="D129" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="130" spans="1:4" s="0" outlineLevel="0">
@@ -2471,7 +2471,7 @@
         <v>1970.00</v>
       </c>
       <c r="D130" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="131" spans="1:4" s="0" outlineLevel="0">
@@ -2535,7 +2535,7 @@
         <v>1970.00</v>
       </c>
       <c r="D134" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="135" spans="1:4" s="0" outlineLevel="0">
@@ -2567,7 +2567,7 @@
         <v>1970.00</v>
       </c>
       <c r="D136" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="137" spans="1:4" s="0" outlineLevel="0">
@@ -2615,7 +2615,7 @@
         <v>1970.00</v>
       </c>
       <c r="D139" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="140" spans="1:4" s="0" outlineLevel="0">
@@ -2647,7 +2647,7 @@
         <v>1970.00</v>
       </c>
       <c r="D141" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="142" spans="1:4" s="0" outlineLevel="0">
@@ -2663,7 +2663,7 @@
         <v>1970.00</v>
       </c>
       <c r="D142" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="143" spans="1:4" s="0" outlineLevel="0">
@@ -2695,7 +2695,7 @@
         <v>1970.00</v>
       </c>
       <c r="D144" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="145" spans="1:4" s="0" outlineLevel="0">
@@ -2823,7 +2823,7 @@
         <v>1970.00</v>
       </c>
       <c r="D152" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="153" spans="1:4" s="0" outlineLevel="0">
@@ -3031,7 +3031,7 @@
         <v>1970.00</v>
       </c>
       <c r="D165" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="166" spans="1:4" s="0" outlineLevel="0">
@@ -3175,7 +3175,7 @@
         <v>1970.00</v>
       </c>
       <c r="D174" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="175" spans="1:4" s="0" outlineLevel="0">
@@ -3383,7 +3383,7 @@
         <v>1970.00</v>
       </c>
       <c r="D187" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="188" spans="1:4" s="0" outlineLevel="0">
@@ -3543,7 +3543,7 @@
         <v>1970.00</v>
       </c>
       <c r="D197" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="198" spans="1:4" s="0" outlineLevel="0">
@@ -3575,7 +3575,7 @@
         <v>1970.00</v>
       </c>
       <c r="D199" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="200" spans="1:4" s="0" outlineLevel="0">
@@ -5031,7 +5031,7 @@
         <v>1970.00</v>
       </c>
       <c r="D290" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="291" spans="1:4" s="0" outlineLevel="0">

</xml_diff>

<commit_message>
nieuwe wijken + correcties
Toevoegen wijken voor (closes #29):
* Knokke-Heist
* Oostkamp
* Menen
* Zwevegem
* Waregem
* Deerlijk
* Oudsbergen
* Langemark-Poelkapelle (verschijnt nu pas in provincies.incijfers.be, maar was reeds toegevoegd in dataset via https://github.com/provinciesincijfers/gebiedsniveaus/commit/3c12f6600957d873e6742fb852195a0c04210e00)

Correctie van de gemeentegedragen wijkcodes van Kortrijk (closes #31). Deze wijkcodes waren abusievelijk van het type "3402234022WJ", het is te zeggen, de niscode van de gemeente stond er twee keer in. Dit is nu rechtgezet naar de normale 34022WJ. Er is géén inhoudelijke aanpassing van deze wijken.

Enkele correcties in statsec namen (closes #30)
</commit_message>
<xml_diff>
--- a/data_voor_swing/uploadfiles/ggw7_type.xlsx
+++ b/data_voor_swing/uploadfiles/ggw7_type.xlsx
@@ -1247,11 +1247,11 @@
         <v>1970.00</v>
       </c>
       <c r="D41" s="8">
-        <v>1.00</v>
+        <v>2.00</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>12035_01</t>
+          <t>12035A0</t>
         </is>
       </c>
     </row>
@@ -3746,11 +3746,11 @@
         <v>1970.00</v>
       </c>
       <c r="D160" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>31022A0</t>
+          <t>31022BAB</t>
         </is>
       </c>
     </row>
@@ -3830,11 +3830,11 @@
         <v>1970.00</v>
       </c>
       <c r="D164" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>31043A0</t>
+          <t>31043DUI</t>
         </is>
       </c>
     </row>
@@ -4082,11 +4082,11 @@
         <v>1970.00</v>
       </c>
       <c r="D176" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>33040A0</t>
+          <t>33040BIKS</t>
         </is>
       </c>
     </row>
@@ -4166,11 +4166,11 @@
         <v>1970.00</v>
       </c>
       <c r="D180" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>34009A0</t>
+          <t>34009BELG</t>
         </is>
       </c>
     </row>
@@ -4212,7 +4212,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>3402234022WA</t>
+          <t>34022WA</t>
         </is>
       </c>
     </row>
@@ -4271,11 +4271,11 @@
         <v>1970.00</v>
       </c>
       <c r="D185" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>34027A0</t>
+          <t>34027BAR</t>
         </is>
       </c>
     </row>
@@ -4292,11 +4292,11 @@
         <v>1970.00</v>
       </c>
       <c r="D186" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>34040A0</t>
+          <t>34040BEVL</t>
         </is>
       </c>
     </row>
@@ -4334,11 +4334,11 @@
         <v>1970.00</v>
       </c>
       <c r="D188" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>34042A0</t>
+          <t>34042CENT</t>
         </is>
       </c>
     </row>
@@ -6812,11 +6812,11 @@
         <v>1970.00</v>
       </c>
       <c r="D306" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>71047A0</t>
+          <t>72042EL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Toevoegen nieuwe wijken najaar 2022
Closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/40
</commit_message>
<xml_diff>
--- a/data_voor_swing/uploadfiles/ggw7_type.xlsx
+++ b/data_voor_swing/uploadfiles/ggw7_type.xlsx
@@ -1499,11 +1499,11 @@
         <v>1970.00</v>
       </c>
       <c r="D53" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>13013A0</t>
+          <t>13013BER</t>
         </is>
       </c>
     </row>
@@ -2339,7 +2339,7 @@
         <v>1970.00</v>
       </c>
       <c r="D93" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2507,7 +2507,7 @@
         <v>1970.00</v>
       </c>
       <c r="D101" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
         <v>1970.00</v>
       </c>
       <c r="D102" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2738,11 +2738,11 @@
         <v>1970.00</v>
       </c>
       <c r="D112" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>23086A0</t>
+          <t>23086B0</t>
         </is>
       </c>
     </row>
@@ -3137,7 +3137,7 @@
         <v>1970.00</v>
       </c>
       <c r="D131" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3326,7 +3326,7 @@
         <v>1970.00</v>
       </c>
       <c r="D140" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3452,7 +3452,7 @@
         <v>1970.00</v>
       </c>
       <c r="D146" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -3494,7 +3494,7 @@
         <v>1970.00</v>
       </c>
       <c r="D148" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -3767,11 +3767,11 @@
         <v>1970.00</v>
       </c>
       <c r="D161" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>31033A0</t>
+          <t>31033CENT</t>
         </is>
       </c>
     </row>
@@ -3977,11 +3977,11 @@
         <v>1970.00</v>
       </c>
       <c r="D171" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>33016A0</t>
+          <t>33016MEB</t>
         </is>
       </c>
     </row>
@@ -4544,11 +4544,11 @@
         <v>1970.00</v>
       </c>
       <c r="D198" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>36007A0</t>
+          <t>36007INGNO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
enkele correcties van wijken + toevoegen Nazareth
Correcties:
- Diksmuide: Keiem, deze keer wel gefixed
- Harelbeke: Centrum was fout (reeds lang bestaande wijkindeling)
- Westerlo: onterecht gesplitste wijk (in een nieuwe wijkindeling)

Toevoeging gemeente Nazareth (kon nog meegenomen worden omwille van het fixen van bovenstaande)
</commit_message>
<xml_diff>
--- a/data_voor_swing/uploadfiles/ggw7_type.xlsx
+++ b/data_voor_swing/uploadfiles/ggw7_type.xlsx
@@ -5720,11 +5720,11 @@
         <v>1970.00</v>
       </c>
       <c r="D254" s="8">
-        <v>2.00</v>
+        <v>1.00</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>44048A0</t>
+          <t>4404801</t>
         </is>
       </c>
     </row>

</xml_diff>